<commit_message>
fix(supplementary-materials): fix wrong chapter count
</commit_message>
<xml_diff>
--- a/supplementary-materials/1838 Titles 1-15.xlsx
+++ b/supplementary-materials/1838 Titles 1-15.xlsx
@@ -199,10 +199,10 @@
     <t xml:space="preserve">James Fraser</t>
   </si>
   <si>
-    <t xml:space="preserve">Intro+5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15812__chp5of6_seed15812.html</t>
+    <t xml:space="preserve">Intro+7+5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15812__collingridge_night_near_windsor_chp13of13_seed15812.html</t>
   </si>
   <si>
     <t xml:space="preserve">Smith</t>
@@ -340,7 +340,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -628,7 +628,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>

</xml_diff>